<commit_message>
Now blancoValueObject v.0.0.1 released!
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557EFF8C-0A5A-7941-BCFC-C06A32038033}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4A5863-A0F6-4F4D-912F-4E78490E37E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="79">
   <si>
     <t>クラス名</t>
   </si>
@@ -472,10 +472,6 @@
     <rPh sb="14" eb="16">
       <t xml:space="preserve">ドクジ </t>
     </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>import {SimpleSample} from "./SimpleSample"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1692,7 +1688,7 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -2356,12 +2352,8 @@
       <c r="O40" s="39"/>
     </row>
     <row r="41" spans="1:15">
-      <c r="A41" s="55">
-        <v>1</v>
-      </c>
-      <c r="B41" s="50" t="s">
-        <v>79</v>
-      </c>
+      <c r="A41" s="55"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="42"/>
       <c r="D41" s="42"/>
       <c r="E41" s="42"/>

</xml_diff>

<commit_message>
Add meta file sample for TypeScript decoration. * meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB484958-E4FA-CD4B-A23D-4AC2F4B8A377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7C90E4-6D64-6D45-A2AF-003A6A1CC2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>クラス名</t>
   </si>
@@ -480,6 +480,24 @@
   </si>
   <si>
     <t>new SimpleSample()</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>デコレーション</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>※ JavaやKotlin向けです</t>
+    <rPh sb="13" eb="14">
+      <t xml:space="preserve">ムケ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>※ TypeScript向けです</t>
+    <rPh sb="12" eb="13">
+      <t xml:space="preserve">ムケデス </t>
+    </rPh>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1093,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1235,11 +1253,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1694,46 +1707,46 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="5" style="1" customWidth="1"/>
-    <col min="2" max="6" width="23.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28" style="1" customWidth="1"/>
-    <col min="14" max="14" width="33.33203125" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="1"/>
+    <col min="2" max="7" width="23.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="28" style="1" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19">
+    <row r="1" spans="1:14" ht="19">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1741,13 +1754,14 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="80"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1757,14 +1771,15 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="81"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
-      <c r="K6" s="39"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="K6" s="38"/>
+      <c r="L6" s="39"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1774,14 +1789,15 @@
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="81"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="38"/>
       <c r="I7" s="38"/>
       <c r="J7" s="38"/>
-      <c r="K7" s="39"/>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1791,33 +1807,35 @@
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="81"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="38"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
-      <c r="K8" s="39"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="83" t="s">
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="84"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="10" t="s">
         <v>75</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="81" t="s">
+      <c r="F9" s="37"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="38"/>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
-      <c r="K9" s="39"/>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="K9" s="38"/>
+      <c r="L9" s="39"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1827,137 +1845,147 @@
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="38"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="38" t="s">
+        <v>82</v>
+      </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="39"/>
-    </row>
-    <row r="11" spans="1:13" ht="29" customHeight="1">
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+    </row>
+    <row r="12" spans="1:14" ht="29" customHeight="1">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="85" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="82"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38"/>
-    </row>
-    <row r="13" spans="1:13" s="33" customFormat="1">
-      <c r="A13" s="66" t="s">
+      <c r="N12" s="38"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+    </row>
+    <row r="14" spans="1:14" s="33" customFormat="1">
+      <c r="A14" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="67"/>
-      <c r="C13" s="68"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="73"/>
-      <c r="K13"/>
-    </row>
-    <row r="14" spans="1:13" s="33" customFormat="1">
-      <c r="A14" s="66" t="s">
-        <v>63</v>
-      </c>
       <c r="B14" s="67"/>
-      <c r="C14" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
-      </c>
+      <c r="C14" s="68"/>
+      <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="70"/>
+      <c r="H14"/>
       <c r="I14" s="70"/>
-      <c r="J14" s="73"/>
-      <c r="K14"/>
-    </row>
-    <row r="15" spans="1:13" s="33" customFormat="1">
+      <c r="J14" s="70"/>
+      <c r="K14" s="73"/>
+      <c r="L14"/>
+    </row>
+    <row r="15" spans="1:14" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" s="67"/>
-      <c r="C15" s="68"/>
-      <c r="D15"/>
+      <c r="C15" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="70"/>
+      <c r="H15"/>
       <c r="I15" s="70"/>
-      <c r="J15" s="73"/>
-      <c r="K15"/>
-    </row>
-    <row r="16" spans="1:13" s="33" customFormat="1">
-      <c r="A16" s="95" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="96"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="73"/>
+      <c r="L15"/>
+    </row>
+    <row r="16" spans="1:14" s="33" customFormat="1">
+      <c r="A16" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="67"/>
       <c r="C16" s="68"/>
-      <c r="D16" t="s">
-        <v>78</v>
-      </c>
+      <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16" s="70"/>
+      <c r="H16"/>
       <c r="I16" s="70"/>
-      <c r="J16" s="73"/>
-      <c r="K16"/>
-    </row>
-    <row r="17" spans="1:15" s="33" customFormat="1">
-      <c r="A17" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="73"/>
+      <c r="L16"/>
+    </row>
+    <row r="17" spans="1:16" s="33" customFormat="1">
+      <c r="A17" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="93"/>
+      <c r="C17" s="68"/>
+      <c r="D17" t="s">
+        <v>78</v>
+      </c>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="70"/>
+      <c r="H17"/>
       <c r="I17" s="70"/>
-      <c r="J17" s="73"/>
-      <c r="K17"/>
-    </row>
-    <row r="18" spans="1:15" s="33" customFormat="1">
+      <c r="J17" s="70"/>
+      <c r="K17" s="73"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:16" s="33" customFormat="1">
       <c r="A18" s="66" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B18" s="67"/>
       <c r="C18" s="68" t="s">
@@ -1967,14 +1995,15 @@
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="H18" s="70"/>
+      <c r="H18"/>
       <c r="I18" s="70"/>
-      <c r="J18" s="73"/>
-      <c r="K18"/>
-    </row>
-    <row r="19" spans="1:15" s="33" customFormat="1">
+      <c r="J18" s="70"/>
+      <c r="K18" s="73"/>
+      <c r="L18"/>
+    </row>
+    <row r="19" spans="1:16" s="33" customFormat="1">
       <c r="A19" s="66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="67"/>
       <c r="C19" s="68" t="s">
@@ -1984,731 +2013,787 @@
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" s="70"/>
+      <c r="H19"/>
       <c r="I19" s="70"/>
-      <c r="J19" s="73"/>
-      <c r="K19"/>
-    </row>
-    <row r="20" spans="1:15" s="33" customFormat="1">
-      <c r="A20" s="95" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="96"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="73"/>
+      <c r="L19"/>
+    </row>
+    <row r="20" spans="1:16" s="33" customFormat="1">
+      <c r="A20" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="67"/>
       <c r="C20" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
+      <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
-      <c r="H20" s="70"/>
+      <c r="H20"/>
       <c r="I20" s="70"/>
-      <c r="J20" s="73"/>
-      <c r="K20"/>
-    </row>
-    <row r="21" spans="1:15" s="41" customFormat="1">
-      <c r="A21" s="38"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22" s="31" t="s">
+      <c r="J20" s="70"/>
+      <c r="K20" s="73"/>
+      <c r="L20"/>
+    </row>
+    <row r="21" spans="1:16" s="33" customFormat="1">
+      <c r="A21" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="93"/>
+      <c r="C21" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="73"/>
+      <c r="L21"/>
+    </row>
+    <row r="22" spans="1:16" s="41" customFormat="1">
+      <c r="A22" s="38"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="33"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="48"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="48"/>
       <c r="M23" s="33"/>
       <c r="N23" s="33"/>
       <c r="O23" s="33"/>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="3" t="s">
+      <c r="P23" s="33"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="39"/>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="38"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="76"/>
       <c r="H25" s="38"/>
       <c r="I25" s="38"/>
       <c r="J25" s="38"/>
-      <c r="K25" s="39"/>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="38"/>
-      <c r="B26" s="40"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="39"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="77"/>
       <c r="H26" s="38"/>
       <c r="I26" s="38"/>
       <c r="J26" s="38"/>
-      <c r="K26" s="39"/>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="31" t="s">
+      <c r="K26" s="38"/>
+      <c r="L26" s="39"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="38"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="39"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="47"/>
-      <c r="M27" s="47"/>
-      <c r="N27" s="47"/>
-      <c r="O27" s="47"/>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="51" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B29" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="39"/>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="55"/>
-      <c r="B29" s="50"/>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="39"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="48"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="49"/>
+      <c r="P29" s="39"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="55"/>
       <c r="B30" s="50"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="72"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="43"/>
       <c r="H30" s="72"/>
       <c r="I30" s="72"/>
       <c r="J30" s="72"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="40"/>
+      <c r="K30" s="72"/>
+      <c r="L30" s="38"/>
       <c r="M30" s="40"/>
       <c r="N30" s="40"/>
-      <c r="O30" s="39"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="56"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="72"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="39"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="55"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="45"/>
       <c r="H31" s="72"/>
       <c r="I31" s="72"/>
       <c r="J31" s="72"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="40"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="38"/>
       <c r="M31" s="40"/>
       <c r="N31" s="40"/>
-      <c r="O31" s="39"/>
-    </row>
-    <row r="32" spans="1:15" s="41" customFormat="1">
-      <c r="A32" s="38"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
-      <c r="K32" s="38"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="39"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="56"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="72"/>
+      <c r="K32" s="72"/>
       <c r="L32" s="38"/>
-      <c r="M32" s="38"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="31" t="s">
+      <c r="M32" s="40"/>
+      <c r="N32" s="40"/>
+      <c r="O32" s="40"/>
+      <c r="P32" s="39"/>
+    </row>
+    <row r="33" spans="1:16" s="41" customFormat="1">
+      <c r="A33" s="38"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="47"/>
-      <c r="M33" s="47"/>
-      <c r="N33" s="47"/>
-      <c r="O33" s="47"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="51" t="s">
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="48"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="46" t="s">
+      <c r="B35" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="39"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="55">
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="48"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="39"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="55">
         <v>1</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B36" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="72"/>
-      <c r="H35" s="72"/>
-      <c r="I35" s="72"/>
-      <c r="J35" s="72"/>
-      <c r="K35" s="38"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="40"/>
-      <c r="N35" s="40"/>
-      <c r="O35" s="39"/>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="55"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="72"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
       <c r="H36" s="72"/>
       <c r="I36" s="72"/>
       <c r="J36" s="72"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="40"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="38"/>
       <c r="M36" s="40"/>
       <c r="N36" s="40"/>
-      <c r="O36" s="39"/>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="56"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="72"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="39"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="55"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="45"/>
       <c r="H37" s="72"/>
       <c r="I37" s="72"/>
       <c r="J37" s="72"/>
-      <c r="K37" s="38"/>
-      <c r="L37" s="40"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="38"/>
       <c r="M37" s="40"/>
       <c r="N37" s="40"/>
-      <c r="O37" s="39"/>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
-      <c r="K38" s="13"/>
-      <c r="L38" s="13"/>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="31" t="s">
+      <c r="O37" s="40"/>
+      <c r="P37" s="39"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="56"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="72"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="40"/>
+      <c r="N38" s="40"/>
+      <c r="O38" s="40"/>
+      <c r="P38" s="39"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="32"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="47"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="47"/>
-      <c r="O39" s="47"/>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="51" t="s">
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="48"/>
+      <c r="L40" s="48"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="47"/>
+      <c r="P40" s="47"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="46" t="s">
+      <c r="B41" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="71"/>
-      <c r="H40" s="71"/>
-      <c r="I40" s="71"/>
-      <c r="J40" s="71"/>
-      <c r="K40" s="71"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="39"/>
-    </row>
-    <row r="41" spans="1:15">
-      <c r="A41" s="55"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="O41" s="39"/>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="39"/>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" s="55"/>
       <c r="B42" s="50"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="72"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="42"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="43"/>
       <c r="H42" s="72"/>
       <c r="I42" s="72"/>
       <c r="J42" s="72"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="40"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="38"/>
       <c r="M42" s="40"/>
       <c r="N42" s="40"/>
-      <c r="O42" s="39"/>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="A43" s="56"/>
-      <c r="B43" s="52"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="72"/>
+      <c r="O42" s="40"/>
+      <c r="P42" s="39"/>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="55"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
       <c r="H43" s="72"/>
       <c r="I43" s="72"/>
       <c r="J43" s="72"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="40"/>
+      <c r="K43" s="72"/>
+      <c r="L43" s="38"/>
       <c r="M43" s="40"/>
       <c r="N43" s="40"/>
-      <c r="O43" s="39"/>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="3" t="s">
+      <c r="O43" s="40"/>
+      <c r="P43" s="39"/>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" s="56"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="72"/>
+      <c r="J44" s="72"/>
+      <c r="K44" s="72"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="40"/>
+      <c r="N44" s="40"/>
+      <c r="O44" s="40"/>
+      <c r="P44" s="39"/>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+      <c r="L45" s="13"/>
+      <c r="M45" s="13"/>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="15"/>
-    </row>
-    <row r="46" spans="1:15" ht="13.5" customHeight="1">
-      <c r="A46" s="89" t="s">
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="N46" s="14"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="15"/>
+    </row>
+    <row r="47" spans="1:16" ht="13.5" customHeight="1">
+      <c r="A47" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="89" t="s">
+      <c r="B47" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="88" t="s">
+      <c r="C47" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="88" t="s">
+      <c r="D47" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E46" s="90" t="s">
+      <c r="E47" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="F46" s="88" t="s">
+      <c r="F47" s="87" t="s">
+        <v>81</v>
+      </c>
+      <c r="G47" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="90" t="s">
+      <c r="H47" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="H46" s="90" t="s">
+      <c r="I47" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="I46" s="93" t="s">
+      <c r="J47" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="J46" s="93" t="s">
+      <c r="K47" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="K46" s="88" t="s">
+      <c r="L47" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="L46" s="88"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="9"/>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" s="89"/>
-      <c r="B47" s="89"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="88"/>
-      <c r="E47" s="91"/>
-      <c r="F47" s="88"/>
-      <c r="G47" s="92"/>
-      <c r="H47" s="92"/>
-      <c r="I47" s="94"/>
-      <c r="J47" s="94"/>
-      <c r="K47" s="88"/>
-      <c r="L47" s="88"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="15"/>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="A48" s="19">
+      <c r="M47" s="85"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="9"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="86"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="85"/>
+      <c r="D48" s="85"/>
+      <c r="E48" s="88"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
+      <c r="H48" s="89"/>
+      <c r="I48" s="89"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="91"/>
+      <c r="L48" s="85"/>
+      <c r="M48" s="85"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="15"/>
+    </row>
+    <row r="49" spans="1:16">
+      <c r="A49" s="19">
         <v>1</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B49" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C49" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G48" s="21"/>
-      <c r="H48" s="78"/>
-      <c r="I48" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="J48" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="K48" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="29"/>
-      <c r="O48" s="15"/>
-    </row>
-    <row r="49" spans="1:15">
-      <c r="A49" s="19">
-        <f>A48+1</f>
-        <v>2</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>54</v>
       </c>
       <c r="D49" s="21"/>
       <c r="E49" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="21">
-        <v>0</v>
-      </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="78"/>
+        <v>55</v>
+      </c>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H49" s="21"/>
       <c r="I49" s="78"/>
       <c r="J49" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="K49" s="21"/>
-      <c r="L49" s="22"/>
+      <c r="K49" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="L49" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="M49" s="22"/>
-      <c r="N49" s="29"/>
-      <c r="O49" s="15"/>
-    </row>
-    <row r="50" spans="1:15">
+      <c r="N49" s="22"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="15"/>
+    </row>
+    <row r="50" spans="1:16">
       <c r="A50" s="19">
-        <f t="shared" ref="A50:A52" si="0">A49+1</f>
-        <v>3</v>
+        <f>A49+1</f>
+        <v>2</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="21"/>
+        <v>54</v>
+      </c>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="78" t="s">
-        <v>45</v>
-      </c>
+      <c r="G50" s="21">
+        <v>0</v>
+      </c>
+      <c r="H50" s="21"/>
       <c r="I50" s="78"/>
       <c r="J50" s="78"/>
-      <c r="K50" s="21" t="s">
+      <c r="K50" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="L50" s="21"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="15"/>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="19">
+        <f t="shared" ref="A51:A53" si="0">A50+1</f>
+        <v>3</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="J51" s="78"/>
+      <c r="K51" s="78"/>
+      <c r="L51" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
-      <c r="N50" s="23"/>
-      <c r="O50" s="15"/>
-    </row>
-    <row r="51" spans="1:15">
-      <c r="A51" s="19">
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="15"/>
+    </row>
+    <row r="52" spans="1:16">
+      <c r="A52" s="19">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B52" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C52" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21" t="s">
+      <c r="D52" s="21"/>
+      <c r="E52" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F52" s="21"/>
+      <c r="G52" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="G51" s="21"/>
-      <c r="H51" s="78"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="78"/>
-      <c r="K51" s="21" t="s">
+      <c r="H52" s="21"/>
+      <c r="I52" s="78"/>
+      <c r="J52" s="78"/>
+      <c r="K52" s="78"/>
+      <c r="L52" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="23"/>
-      <c r="O51" s="15"/>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="A52" s="19">
+      <c r="M52" s="22"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="23"/>
+      <c r="P52" s="15"/>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B53" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C53" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21" t="s">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="F53" s="21"/>
+      <c r="G53" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G52" s="21"/>
-      <c r="H52" s="78"/>
-      <c r="I52" s="78"/>
-      <c r="J52" s="78"/>
-      <c r="K52" s="21" t="s">
+      <c r="H53" s="21"/>
+      <c r="I53" s="78"/>
+      <c r="J53" s="78"/>
+      <c r="K53" s="78"/>
+      <c r="L53" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="L52" s="22"/>
-      <c r="M52" s="22"/>
-      <c r="N52" s="23"/>
-      <c r="O52" s="15"/>
-    </row>
-    <row r="53" spans="1:15">
-      <c r="A53" s="24"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="79"/>
-      <c r="I53" s="79"/>
-      <c r="J53" s="79"/>
-      <c r="K53" s="26"/>
-      <c r="L53" s="27"/>
-      <c r="M53" s="27"/>
-      <c r="N53" s="28"/>
-      <c r="O53" s="15"/>
+      <c r="M53" s="22"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="23"/>
+      <c r="P53" s="15"/>
+    </row>
+    <row r="54" spans="1:16">
+      <c r="A54" s="24"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="26"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="26"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
+      <c r="O54" s="28"/>
+      <c r="P54" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K46:L47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="J46:J47"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="L47:M48"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="F47:F48"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F69:J69" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G70:K70" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C20" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C21" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G48:G53 C15:C16" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H49:H54 C16:C17" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
       <formula1>isFinal</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
       <formula1>isData</formula1>
     </dataValidation>
   </dataValidations>
@@ -2724,7 +2809,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H48:J53</xm:sqref>
+          <xm:sqref>I49:K54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
0.0.10: Enable alias for class name, for listClass property.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
+++ b/meta/objects/BlancoValueObjectTsAnnotationSample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7C90E4-6D64-6D45-A2AF-003A6A1CC2ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002DDFF0-77D6-F346-B501-20020B826B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="87">
   <si>
     <t>クラス名</t>
   </si>
@@ -497,6 +497,33 @@
     <t>※ TypeScript向けです</t>
     <rPh sb="12" eb="13">
       <t xml:space="preserve">ムケデス </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>エイリアス名</t>
+    <rPh sb="5" eb="6">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>annotationSample</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>※ listClassが指定された場合にプロパティ名に使われます。</t>
+    <rPh sb="12" eb="14">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t xml:space="preserve">バアイニ </t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t xml:space="preserve">メイニ </t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t xml:space="preserve">ツカワレマス。 </t>
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
@@ -1278,10 +1305,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1707,10 +1734,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F57" sqref="F57"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1799,56 +1826,56 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="38"/>
+      <c r="H8" s="38" t="s">
+        <v>86</v>
+      </c>
       <c r="I8" s="38"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38"/>
       <c r="L8" s="39"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="80" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="81"/>
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="11"/>
-      <c r="H9" s="38" t="s">
-        <v>76</v>
-      </c>
+      <c r="H9" s="38"/>
       <c r="I9" s="38"/>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
       <c r="L9" s="39"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="6"/>
+      <c r="A10" s="80" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="81"/>
       <c r="C10" s="10" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="11"/>
       <c r="H10" s="38" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
@@ -1857,89 +1884,89 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
       <c r="F11" s="37"/>
       <c r="G11" s="11"/>
       <c r="H11" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="38"/>
       <c r="J11" s="38"/>
       <c r="K11" s="38"/>
       <c r="L11" s="39"/>
     </row>
-    <row r="12" spans="1:14" ht="29" customHeight="1">
+    <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
+    </row>
+    <row r="13" spans="1:14" ht="29" customHeight="1">
+      <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="82" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="38"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="38"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38"/>
       <c r="N13" s="38"/>
     </row>
-    <row r="14" spans="1:14" s="33" customFormat="1">
-      <c r="A14" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="67"/>
-      <c r="C14" s="68"/>
-      <c r="D14"/>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="K14" s="73"/>
-      <c r="L14"/>
+    <row r="14" spans="1:14">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
     </row>
     <row r="15" spans="1:14" s="33" customFormat="1">
       <c r="A15" s="66" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B15" s="67"/>
-      <c r="C15" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
+      <c r="C15" s="68"/>
+      <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
@@ -1951,11 +1978,15 @@
     </row>
     <row r="16" spans="1:14" s="33" customFormat="1">
       <c r="A16" s="66" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B16" s="67"/>
-      <c r="C16" s="68"/>
-      <c r="D16"/>
+      <c r="C16" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
@@ -1966,14 +1997,12 @@
       <c r="L16"/>
     </row>
     <row r="17" spans="1:16" s="33" customFormat="1">
-      <c r="A17" s="92" t="s">
-        <v>77</v>
-      </c>
-      <c r="B17" s="93"/>
+      <c r="A17" s="66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="67"/>
       <c r="C17" s="68"/>
-      <c r="D17" t="s">
-        <v>78</v>
-      </c>
+      <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17"/>
@@ -1984,14 +2013,14 @@
       <c r="L17"/>
     </row>
     <row r="18" spans="1:16" s="33" customFormat="1">
-      <c r="A18" s="66" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="68" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18"/>
+      <c r="A18" s="92" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="93"/>
+      <c r="C18" s="68"/>
+      <c r="D18" t="s">
+        <v>78</v>
+      </c>
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
@@ -2003,7 +2032,7 @@
     </row>
     <row r="19" spans="1:16" s="33" customFormat="1">
       <c r="A19" s="66" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B19" s="67"/>
       <c r="C19" s="68" t="s">
@@ -2021,7 +2050,7 @@
     </row>
     <row r="20" spans="1:16" s="33" customFormat="1">
       <c r="A20" s="66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="67"/>
       <c r="C20" s="68" t="s">
@@ -2038,16 +2067,14 @@
       <c r="L20"/>
     </row>
     <row r="21" spans="1:16" s="33" customFormat="1">
-      <c r="A21" s="92" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" s="93"/>
+      <c r="A21" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="67"/>
       <c r="C21" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="D21" t="s">
-        <v>73</v>
-      </c>
+      <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
@@ -2057,88 +2084,92 @@
       <c r="K21" s="73"/>
       <c r="L21"/>
     </row>
-    <row r="22" spans="1:16" s="41" customFormat="1">
-      <c r="A22" s="38"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="31" t="s">
+    <row r="22" spans="1:16" s="33" customFormat="1">
+      <c r="A22" s="92" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="93"/>
+      <c r="C22" s="68" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
+      <c r="K22" s="73"/>
+      <c r="L22"/>
+    </row>
+    <row r="23" spans="1:16" s="41" customFormat="1">
+      <c r="A23" s="38"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="48"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
       <c r="M24" s="33"/>
       <c r="N24" s="33"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="39"/>
+      <c r="A25" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="77"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="76"/>
       <c r="H26" s="38"/>
       <c r="I26" s="38"/>
       <c r="J26" s="38"/>
@@ -2146,13 +2177,15 @@
       <c r="L26" s="39"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="38"/>
-      <c r="B27" s="40"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
+      <c r="A27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="77"/>
       <c r="H27" s="38"/>
       <c r="I27" s="38"/>
       <c r="J27" s="38"/>
@@ -2160,73 +2193,69 @@
       <c r="L27" s="39"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="38"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="39"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="47"/>
-      <c r="N28" s="47"/>
-      <c r="O28" s="47"/>
-      <c r="P28" s="47"/>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="51" t="s">
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="48"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="48"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="48"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="47"/>
+      <c r="P29" s="47"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="46" t="s">
+      <c r="B30" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="71"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="71"/>
-      <c r="K29" s="71"/>
-      <c r="L29" s="71"/>
-      <c r="M29" s="48"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="39"/>
-    </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="55"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="72"/>
-      <c r="K30" s="72"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40"/>
-      <c r="O30" s="40"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="49"/>
+      <c r="O30" s="49"/>
       <c r="P30" s="39"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="55"/>
       <c r="B31" s="50"/>
-      <c r="C31" s="44"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="45"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="43"/>
       <c r="H31" s="72"/>
       <c r="I31" s="72"/>
       <c r="J31" s="72"/>
@@ -2238,13 +2267,13 @@
       <c r="P31" s="39"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="56"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-      <c r="F32" s="53"/>
-      <c r="G32" s="54"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="45"/>
       <c r="H32" s="72"/>
       <c r="I32" s="72"/>
       <c r="J32" s="72"/>
@@ -2255,94 +2284,94 @@
       <c r="O32" s="40"/>
       <c r="P32" s="39"/>
     </row>
-    <row r="33" spans="1:16" s="41" customFormat="1">
-      <c r="A33" s="38"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
+    <row r="33" spans="1:16">
+      <c r="A33" s="56"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
       <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
-    </row>
-    <row r="34" spans="1:16">
-      <c r="A34" s="31" t="s">
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="39"/>
+    </row>
+    <row r="34" spans="1:16" s="41" customFormat="1">
+      <c r="A34" s="38"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="38"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="47"/>
-    </row>
-    <row r="35" spans="1:16">
-      <c r="A35" s="51" t="s">
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="48"/>
+      <c r="I35" s="48"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="48"/>
+      <c r="L35" s="48"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="47"/>
+      <c r="P35" s="47"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B36" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="71"/>
-      <c r="M35" s="48"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="39"/>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="55">
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="71"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="49"/>
+      <c r="P36" s="39"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="55">
         <v>1</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B37" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="40"/>
-      <c r="N36" s="40"/>
-      <c r="O36" s="40"/>
-      <c r="P36" s="39"/>
-    </row>
-    <row r="37" spans="1:16">
-      <c r="A37" s="55"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="45"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="43"/>
       <c r="H37" s="72"/>
       <c r="I37" s="72"/>
       <c r="J37" s="72"/>
@@ -2354,13 +2383,13 @@
       <c r="P37" s="39"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="56"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="54"/>
+      <c r="A38" s="55"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="45"/>
       <c r="H38" s="72"/>
       <c r="I38" s="72"/>
       <c r="J38" s="72"/>
@@ -2372,88 +2401,88 @@
       <c r="P38" s="39"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-      <c r="M39" s="13"/>
+      <c r="A39" s="56"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="72"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="40"/>
+      <c r="N39" s="40"/>
+      <c r="O39" s="40"/>
+      <c r="P39" s="39"/>
     </row>
     <row r="40" spans="1:16">
-      <c r="A40" s="31" t="s">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13"/>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="B40" s="32"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="48"/>
-      <c r="M40" s="47"/>
-      <c r="N40" s="47"/>
-      <c r="O40" s="47"/>
-      <c r="P40" s="47"/>
-    </row>
-    <row r="41" spans="1:16">
-      <c r="A41" s="51" t="s">
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="47"/>
+      <c r="P41" s="47"/>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="A42" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="46" t="s">
+      <c r="B42" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="71"/>
-      <c r="L41" s="71"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="39"/>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" s="55"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="43"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="48"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
       <c r="P42" s="39"/>
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="55"/>
       <c r="B43" s="50"/>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
-      <c r="G43" s="45"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
       <c r="H43" s="72"/>
       <c r="I43" s="72"/>
       <c r="J43" s="72"/>
@@ -2465,13 +2494,13 @@
       <c r="P43" s="39"/>
     </row>
     <row r="44" spans="1:16">
-      <c r="A44" s="56"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="54"/>
+      <c r="A44" s="55"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="44"/>
+      <c r="G44" s="45"/>
       <c r="H44" s="72"/>
       <c r="I44" s="72"/>
       <c r="J44" s="72"/>
@@ -2483,160 +2512,147 @@
       <c r="P44" s="39"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="13"/>
-      <c r="L45" s="13"/>
-      <c r="M45" s="13"/>
+      <c r="A45" s="56"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="38"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="40"/>
+      <c r="O45" s="40"/>
+      <c r="P45" s="39"/>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="14"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="15"/>
-    </row>
-    <row r="47" spans="1:16" ht="13.5" customHeight="1">
-      <c r="A47" s="86" t="s">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="15"/>
+    </row>
+    <row r="48" spans="1:16" ht="13.5" customHeight="1">
+      <c r="A48" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="86" t="s">
+      <c r="B48" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="85" t="s">
+      <c r="C48" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="85" t="s">
+      <c r="D48" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="E47" s="87" t="s">
+      <c r="E48" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="F47" s="87" t="s">
+      <c r="F48" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="G47" s="87" t="s">
+      <c r="G48" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="H47" s="87" t="s">
+      <c r="H48" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="I47" s="87" t="s">
+      <c r="I48" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="J47" s="90" t="s">
+      <c r="J48" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="K47" s="90" t="s">
+      <c r="K48" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="L47" s="85" t="s">
+      <c r="L48" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="M47" s="85"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="9"/>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" s="86"/>
-      <c r="B48" s="86"/>
-      <c r="C48" s="85"/>
-      <c r="D48" s="85"/>
-      <c r="E48" s="88"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="89"/>
-      <c r="H48" s="89"/>
-      <c r="I48" s="89"/>
-      <c r="J48" s="91"/>
-      <c r="K48" s="91"/>
-      <c r="L48" s="85"/>
       <c r="M48" s="85"/>
-      <c r="N48" s="18"/>
-      <c r="O48" s="30"/>
-      <c r="P48" s="15"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="9"/>
     </row>
     <row r="49" spans="1:16">
-      <c r="A49" s="19">
-        <v>1</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H49" s="21"/>
-      <c r="I49" s="78"/>
-      <c r="J49" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="K49" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="L49" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="M49" s="22"/>
-      <c r="N49" s="22"/>
-      <c r="O49" s="29"/>
+      <c r="A49" s="86"/>
+      <c r="B49" s="86"/>
+      <c r="C49" s="85"/>
+      <c r="D49" s="85"/>
+      <c r="E49" s="89"/>
+      <c r="F49" s="88"/>
+      <c r="G49" s="88"/>
+      <c r="H49" s="88"/>
+      <c r="I49" s="88"/>
+      <c r="J49" s="91"/>
+      <c r="K49" s="91"/>
+      <c r="L49" s="85"/>
+      <c r="M49" s="85"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="30"/>
       <c r="P49" s="15"/>
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="19">
-        <f>A49+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D50" s="21"/>
       <c r="E50" s="21" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F50" s="21"/>
-      <c r="G50" s="21">
-        <v>0</v>
+      <c r="G50" s="21" t="s">
+        <v>34</v>
       </c>
       <c r="H50" s="21"/>
       <c r="I50" s="78"/>
-      <c r="J50" s="78"/>
+      <c r="J50" s="78" t="s">
+        <v>45</v>
+      </c>
       <c r="K50" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="L50" s="21"/>
+      <c r="L50" s="21" t="s">
+        <v>13</v>
+      </c>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="29"/>
@@ -2644,60 +2660,60 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" s="19">
-        <f t="shared" ref="A51:A53" si="0">A50+1</f>
-        <v>3</v>
+        <f>A50+1</f>
+        <v>2</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="21"/>
+        <v>54</v>
+      </c>
+      <c r="D51" s="21"/>
+      <c r="E51" s="21" t="s">
+        <v>49</v>
+      </c>
       <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
+      <c r="G51" s="21">
+        <v>0</v>
+      </c>
       <c r="H51" s="21"/>
-      <c r="I51" s="78" t="s">
+      <c r="I51" s="78"/>
+      <c r="J51" s="78"/>
+      <c r="K51" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="J51" s="78"/>
-      <c r="K51" s="78"/>
-      <c r="L51" s="21" t="s">
-        <v>18</v>
-      </c>
+      <c r="L51" s="21"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
-      <c r="O51" s="23"/>
+      <c r="O51" s="29"/>
       <c r="P51" s="15"/>
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" ref="A52:A54" si="0">A51+1</f>
+        <v>3</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D52" s="21"/>
-      <c r="E52" s="21" t="s">
-        <v>47</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="21"/>
       <c r="F52" s="21"/>
-      <c r="G52" s="21" t="s">
-        <v>79</v>
-      </c>
+      <c r="G52" s="21"/>
       <c r="H52" s="21"/>
-      <c r="I52" s="78"/>
+      <c r="I52" s="78" t="s">
+        <v>45</v>
+      </c>
       <c r="J52" s="78"/>
       <c r="K52" s="78"/>
       <c r="L52" s="21" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
@@ -2707,28 +2723,28 @@
     <row r="53" spans="1:16">
       <c r="A53" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D53" s="21"/>
       <c r="E53" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F53" s="21"/>
       <c r="G53" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H53" s="21"/>
       <c r="I53" s="78"/>
       <c r="J53" s="78"/>
       <c r="K53" s="78"/>
       <c r="L53" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
@@ -2736,64 +2752,95 @@
       <c r="P53" s="15"/>
     </row>
     <row r="54" spans="1:16">
-      <c r="A54" s="24"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
-      <c r="I54" s="79"/>
-      <c r="J54" s="79"/>
-      <c r="K54" s="79"/>
-      <c r="L54" s="26"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="27"/>
-      <c r="O54" s="28"/>
+      <c r="A54" s="19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H54" s="21"/>
+      <c r="I54" s="78"/>
+      <c r="J54" s="78"/>
+      <c r="K54" s="78"/>
+      <c r="L54" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="M54" s="22"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="23"/>
       <c r="P54" s="15"/>
+    </row>
+    <row r="55" spans="1:16">
+      <c r="A55" s="24"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="79"/>
+      <c r="J55" s="79"/>
+      <c r="K55" s="79"/>
+      <c r="L55" s="26"/>
+      <c r="M55" s="27"/>
+      <c r="N55" s="27"/>
+      <c r="O55" s="28"/>
+      <c r="P55" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="L47:M48"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="K47:K48"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="H47:H48"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="L48:M49"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F48:F49"/>
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G70:K70" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G71:K71" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20:C21" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21:C22" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{643F6C9A-8760-224C-A7F5-6893BC2E6C68}">
       <formula1>createToString</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>accessScope2</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H49:H54 C16:C17" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H50:H55 C17:C18" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>isAbstract</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{061A2328-C320-074B-A7A0-1D5ADA23E625}">
       <formula1>isFinal</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{2D8A5CB0-577F-DA47-9664-36C261082ADA}">
       <formula1>isData</formula1>
     </dataValidation>
   </dataValidations>
@@ -2809,7 +2856,7 @@
           <x14:formula1>
             <xm:f>config!$P$4:$P$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I49:K54</xm:sqref>
+          <xm:sqref>I50:K55</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>